<commit_message>
TPO 2 -> 28/02/2019
</commit_message>
<xml_diff>
--- a/TOEFL.xlsx
+++ b/TOEFL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd\Desktop\TOFEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd\Desktop\TOEFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="228">
   <si>
     <t>listening</t>
   </si>
@@ -2954,9 +2954,6 @@
     <t>10/14</t>
   </si>
   <si>
-    <t>7-10/14</t>
-  </si>
-  <si>
     <t>vigorously support or defend the cause of.
 "he championed the rights of the working class and the poor"</t>
   </si>
@@ -2997,6 +2994,12 @@
   </si>
   <si>
     <t>4/6</t>
+  </si>
+  <si>
+    <t>11/13</t>
+  </si>
+  <si>
+    <t>6/6</t>
   </si>
 </sst>
 </file>
@@ -5592,8 +5595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:AM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5680,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F4" s="33" t="s">
         <v>213</v>
@@ -5698,10 +5701,10 @@
         <v>211</v>
       </c>
       <c r="K4" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="L4" s="33" t="s">
         <v>225</v>
-      </c>
-      <c r="L4" s="33" t="s">
-        <v>226</v>
       </c>
       <c r="M4" s="32" t="s">
         <v>209</v>
@@ -5715,30 +5718,50 @@
       <c r="P4" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="32"/>
+      <c r="Q4" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="S4" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="T4" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="U4" s="32"/>
+      <c r="U4" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="V4"/>
     </row>
     <row r="5" spans="4:39" x14ac:dyDescent="0.25">
       <c r="D5" s="32">
         <v>2</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>226</v>
+      </c>
       <c r="F5" s="32"/>
       <c r="G5" s="33"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="32"/>
+      <c r="H5" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>227</v>
+      </c>
       <c r="K5" s="33"/>
       <c r="L5" s="32"/>
       <c r="M5" s="33"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="O5" s="33" t="s">
+        <v>212</v>
+      </c>
       <c r="P5" s="32" t="s">
         <v>212</v>
       </c>
@@ -6101,7 +6124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -6250,42 +6273,42 @@
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tpo3 Reading + listening done 15/3/2019
</commit_message>
<xml_diff>
--- a/TOEFL.xlsx
+++ b/TOEFL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="cheetsheet" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="245">
   <si>
     <t>listening</t>
   </si>
@@ -3006,6 +3006,63 @@
   </si>
   <si>
     <t>9/13</t>
+  </si>
+  <si>
+    <t>11/14</t>
+  </si>
+  <si>
+    <t>integral</t>
+  </si>
+  <si>
+    <t>necessary to make a whole complete; essential or fundamental.
+"games are an integral part of the school's curriculum"
+synonyms: essential, fundamental,</t>
+  </si>
+  <si>
+    <t>11/15</t>
+  </si>
+  <si>
+    <t>ensuing</t>
+  </si>
+  <si>
+    <t>happen or occur afterwards or as a result.
+"the difficulties which ensued from their commitment to Cuba"
+synonyms: result, follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">never done or known before.
+"the government took the unprecedented step of releasing confidential correspondence"
+synonyms: unparalleled, unequalled, unmatched, unrivalled, without parallel, without equal; More
+antonyms: normal, common
+</t>
+  </si>
+  <si>
+    <t>unprecedented</t>
+  </si>
+  <si>
+    <t>precedent</t>
+  </si>
+  <si>
+    <t>an earlier event or action that is regarded as an example or guide to be considered in subsequent similar circumstances.
+"there are substantial precedents for using interactive media in training"
+synonyms: model, exemplar, example, pattern</t>
+  </si>
+  <si>
+    <t>virtually</t>
+  </si>
+  <si>
+    <t>reading Score</t>
+  </si>
+  <si>
+    <t>Listening score</t>
+  </si>
+  <si>
+    <t>13/14</t>
+  </si>
+  <si>
+    <t>nearly; almost.
+"the disease destroyed virtually all the vineyards in Orange County"
+synonyms: in effect, effectively, all but, more or less, practically, almost, nearly</t>
   </si>
 </sst>
 </file>
@@ -3625,8 +3682,131 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" xfId="25" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" xfId="21" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="17" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="27" borderId="0" xfId="25" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3636,25 +3816,7 @@
     <xf numFmtId="0" fontId="20" fillId="23" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" xfId="17" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3669,15 +3831,9 @@
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="17" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3702,106 +3858,7 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="0" xfId="22" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" xfId="21" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" xfId="21" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" xfId="17" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" xfId="20" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="7" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="9" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="10" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="16" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="18" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" xfId="25" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4139,708 +4196,708 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="G1" s="49" t="s">
+      <c r="C1" s="38"/>
+      <c r="G1" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="49"/>
+      <c r="H1" s="38"/>
       <c r="N1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
     </row>
     <row r="2" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
     </row>
     <row r="3" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="34" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="51" t="s">
+      <c r="O3" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
     </row>
     <row r="4" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B4" s="51"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="51"/>
-      <c r="P4" s="86" t="s">
+      <c r="O4" s="34"/>
+      <c r="P4" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B5" s="51"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="51"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="43" t="s">
+      <c r="O5" s="34"/>
+      <c r="P5" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="Q5" s="43"/>
-      <c r="R5" s="43"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B6" s="51"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="51"/>
+      <c r="G6" s="34"/>
       <c r="H6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="O6" s="51"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="87"/>
-      <c r="R6" s="87"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
     </row>
     <row r="7" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B7" s="51"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="51"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="51"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
     </row>
     <row r="8" spans="2:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="51"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="51"/>
+      <c r="G8" s="34"/>
       <c r="H8" s="14"/>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="P8" s="69" t="s">
+      <c r="P8" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="Q8" s="44" t="s">
+      <c r="Q8" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="R8" s="68" t="s">
+      <c r="R8" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="S8" s="44" t="s">
+      <c r="S8" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="35" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="35" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O9" s="49"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="44"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="40"/>
     </row>
     <row r="10" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B10" s="43"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="43"/>
+      <c r="G10" s="35"/>
       <c r="H10" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="O10" s="49"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="44"/>
-      <c r="Z10" s="51" t="s">
+      <c r="O10" s="38"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="40"/>
+      <c r="Z10" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="AA10" s="43" t="s">
+      <c r="AA10" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="35"/>
     </row>
     <row r="11" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="43"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="O11" s="49"/>
-      <c r="P11" s="42" t="s">
+      <c r="O11" s="38"/>
+      <c r="P11" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="Q11" s="49" t="s">
+      <c r="Q11" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R11" s="42" t="s">
+      <c r="R11" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="S11" s="49" t="s">
+      <c r="S11" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="Z11" s="51"/>
-      <c r="AA11" s="86" t="s">
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="AB11" s="87"/>
-      <c r="AC11" s="87"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="37"/>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B12" s="43"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="43"/>
+      <c r="G12" s="35"/>
       <c r="H12" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="O12" s="49"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="49"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="49"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="43" t="s">
+      <c r="O12" s="38"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="38"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="AB12" s="43"/>
-      <c r="AC12" s="43"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="35"/>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B13" s="43"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="43"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="18"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="69" t="s">
+      <c r="O13" s="38"/>
+      <c r="P13" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="70" t="s">
+      <c r="Q13" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="R13" s="68" t="s">
+      <c r="R13" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="S13" s="44" t="s">
+      <c r="S13" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="Z13" s="51"/>
-      <c r="AA13" s="86" t="s">
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="AB13" s="87"/>
-      <c r="AC13" s="87"/>
+      <c r="AB13" s="37"/>
+      <c r="AC13" s="37"/>
     </row>
     <row r="14" spans="2:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="43"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="43"/>
+      <c r="G14" s="35"/>
       <c r="H14" s="18"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="44"/>
-      <c r="Z14" s="51"/>
-      <c r="AA14" s="43" t="s">
+      <c r="O14" s="38"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="40"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="AB14" s="43"/>
-      <c r="AC14" s="43"/>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="35"/>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B15" s="43"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="43"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="18"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="44"/>
-      <c r="Z15" s="49" t="s">
+      <c r="O15" s="38"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="40"/>
+      <c r="Z15" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AA15" s="69" t="s">
+      <c r="AA15" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AB15" s="44" t="s">
+      <c r="AB15" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="AC15" s="68" t="s">
+      <c r="AC15" s="41" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B16" s="43"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="43"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="18"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="68" t="s">
+      <c r="O16" s="38"/>
+      <c r="P16" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="42" t="s">
+      <c r="Q16" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="R16" s="44" t="s">
+      <c r="R16" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="Z16" s="49"/>
-      <c r="AA16" s="69"/>
-      <c r="AB16" s="44"/>
-      <c r="AC16" s="68"/>
+      <c r="Z16" s="38"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="40"/>
+      <c r="AC16" s="41"/>
     </row>
     <row r="17" spans="2:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="43"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="43"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="18"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="68"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="44"/>
-      <c r="Z17" s="49"/>
-      <c r="AA17" s="69"/>
-      <c r="AB17" s="44"/>
-      <c r="AC17" s="68"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="41"/>
+      <c r="Q17" s="73"/>
+      <c r="R17" s="40"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="39"/>
+      <c r="AB17" s="40"/>
+      <c r="AC17" s="41"/>
     </row>
     <row r="18" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="43"/>
+      <c r="G18" s="35"/>
       <c r="H18" s="19"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="44"/>
-      <c r="Z18" s="49"/>
-      <c r="AA18" s="51" t="s">
+      <c r="O18" s="38"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="73"/>
+      <c r="R18" s="40"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="AB18" s="51"/>
-      <c r="AC18" s="51"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
     </row>
     <row r="19" spans="2:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G19" s="51" t="s">
+      <c r="G19" s="34" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="O19" s="49"/>
-      <c r="P19" s="51" t="s">
+      <c r="O19" s="38"/>
+      <c r="P19" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="Z19" s="49"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
     </row>
     <row r="20" spans="2:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
-      <c r="G20" s="51"/>
+      <c r="G20" s="34"/>
       <c r="H20" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="O20" s="49"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="Z20" s="49"/>
-      <c r="AA20" s="69" t="s">
+      <c r="O20" s="38"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="AB20" s="44" t="s">
+      <c r="AB20" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="AC20" s="68" t="s">
+      <c r="AC20" s="41" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:29" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G21" s="51"/>
+      <c r="G21" s="34"/>
       <c r="H21" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="O21" s="49"/>
-      <c r="P21" s="69" t="s">
+      <c r="O21" s="38"/>
+      <c r="P21" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="R21" s="68" t="s">
+      <c r="R21" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="Z21" s="49"/>
-      <c r="AA21" s="69"/>
-      <c r="AB21" s="44"/>
-      <c r="AC21" s="68"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="39"/>
+      <c r="AB21" s="40"/>
+      <c r="AC21" s="41"/>
     </row>
     <row r="22" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G22" s="51"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="O22" s="49"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="68"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="69"/>
-      <c r="AB22" s="44"/>
-      <c r="AC22" s="68"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="41"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="39"/>
+      <c r="AB22" s="40"/>
+      <c r="AC22" s="41"/>
     </row>
     <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G23" s="51"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="13"/>
-      <c r="O23" s="49"/>
-      <c r="P23" s="69"/>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="68"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="41"/>
     </row>
     <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G24" s="51"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="14"/>
-      <c r="O24" s="43" t="s">
+      <c r="O24" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="P24" s="49" t="s">
+      <c r="P24" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="Q24" s="90" t="s">
+      <c r="Q24" s="45" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G25" s="43" t="s">
+      <c r="G25" s="35" t="s">
         <v>8</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O25" s="43"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="90"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="45"/>
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G26" s="43"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="43"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="90"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="45"/>
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G27" s="43"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="91" t="s">
+      <c r="O27" s="35"/>
+      <c r="P27" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="Q27" s="90"/>
+      <c r="Q27" s="45"/>
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G28" s="43"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O28" s="43"/>
-      <c r="P28" s="91"/>
-      <c r="Q28" s="90"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="45"/>
     </row>
     <row r="29" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G29" s="43"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="18"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="91"/>
-      <c r="Q29" s="90"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="47"/>
+      <c r="Q29" s="45"/>
     </row>
     <row r="30" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G30" s="43"/>
+      <c r="G30" s="35"/>
       <c r="H30" s="18"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="38" t="s">
+      <c r="O30" s="35"/>
+      <c r="P30" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="Q30" s="44" t="s">
+      <c r="Q30" s="40" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G31" s="43"/>
+      <c r="G31" s="35"/>
       <c r="H31" s="18"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="44"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="40"/>
     </row>
     <row r="32" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="G32" s="43"/>
+      <c r="G32" s="35"/>
       <c r="H32" s="18"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="44"/>
+      <c r="O32" s="35"/>
+      <c r="P32" s="46"/>
+      <c r="Q32" s="40"/>
     </row>
     <row r="33" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G33" s="43"/>
+      <c r="G33" s="35"/>
       <c r="H33" s="18"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="52" t="s">
+      <c r="O33" s="35"/>
+      <c r="P33" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="Q33" s="53" t="s">
+      <c r="Q33" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="R33" s="45"/>
-      <c r="S33" s="54"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="87"/>
     </row>
     <row r="34" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G34" s="43"/>
+      <c r="G34" s="35"/>
       <c r="H34" s="19"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="46"/>
-      <c r="S34" s="56"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="85"/>
+      <c r="Q34" s="88"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="89"/>
     </row>
     <row r="35" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G35" s="41" t="s">
+      <c r="G35" s="58" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="O35" s="43"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="46"/>
-      <c r="S35" s="56"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="85"/>
+      <c r="Q35" s="88"/>
+      <c r="R35" s="81"/>
+      <c r="S35" s="89"/>
     </row>
     <row r="36" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G36" s="41"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="O36" s="43"/>
-      <c r="P36" s="52"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="56"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="85"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="81"/>
+      <c r="S36" s="89"/>
     </row>
     <row r="37" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G37" s="41"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="O37" s="43"/>
-      <c r="P37" s="52"/>
-      <c r="Q37" s="57"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="59"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="85"/>
+      <c r="Q37" s="90"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="92"/>
     </row>
     <row r="38" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G38" s="41"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O38" s="43"/>
-      <c r="P38" s="42" t="s">
+      <c r="O38" s="35"/>
+      <c r="P38" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="Q38" s="60" t="s">
+      <c r="Q38" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="R38" s="60"/>
-      <c r="S38" s="60"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
     </row>
     <row r="39" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G39" s="41"/>
+      <c r="G39" s="58"/>
       <c r="H39" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="O39" s="43"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="51"/>
-      <c r="S39" s="51"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
     </row>
     <row r="40" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G40" s="41"/>
+      <c r="G40" s="58"/>
       <c r="H40" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="O40" s="43"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="49" t="s">
+      <c r="O40" s="35"/>
+      <c r="P40" s="73"/>
+      <c r="Q40" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
     </row>
     <row r="41" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G41" s="41"/>
+      <c r="G41" s="58"/>
       <c r="H41" s="21"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="73"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
+      <c r="S41" s="38"/>
     </row>
     <row r="42" spans="7:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G42" s="41"/>
-      <c r="H42" s="80" t="s">
+      <c r="G42" s="58"/>
+      <c r="H42" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="O42" s="43"/>
-      <c r="P42" s="49" t="s">
+      <c r="O42" s="35"/>
+      <c r="P42" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q42" s="60" t="s">
+      <c r="Q42" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="R42" s="60"/>
-      <c r="S42" s="60"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
     </row>
     <row r="43" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G43" s="41"/>
-      <c r="H43" s="81"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="51"/>
-      <c r="R43" s="51"/>
-      <c r="S43" s="51"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="63"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="34"/>
+      <c r="R43" s="34"/>
+      <c r="S43" s="34"/>
     </row>
     <row r="44" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G44" s="41"/>
-      <c r="H44" s="81"/>
-      <c r="O44" s="43"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="61" t="s">
+      <c r="G44" s="58"/>
+      <c r="H44" s="63"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="93" t="s">
         <v>156</v>
       </c>
-      <c r="R44" s="61"/>
-      <c r="S44" s="61"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
     </row>
     <row r="45" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G45" s="41"/>
-      <c r="H45" s="81"/>
-      <c r="O45" s="43"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="61"/>
-      <c r="R45" s="61"/>
-      <c r="S45" s="61"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="63"/>
+      <c r="O45" s="35"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="93"/>
+      <c r="R45" s="93"/>
+      <c r="S45" s="93"/>
     </row>
     <row r="46" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G46" s="41"/>
-      <c r="H46" s="81"/>
-      <c r="O46" s="47" t="s">
+      <c r="G46" s="58"/>
+      <c r="H46" s="63"/>
+      <c r="O46" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="P46" s="44" t="s">
+      <c r="P46" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="Q46" s="44"/>
-      <c r="R46" s="44"/>
-      <c r="S46" s="44"/>
+      <c r="Q46" s="40"/>
+      <c r="R46" s="40"/>
+      <c r="S46" s="40"/>
     </row>
     <row r="47" spans="7:19" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G47" s="51" t="s">
+      <c r="G47" s="34" t="s">
         <v>32</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="O47" s="47"/>
-      <c r="P47" s="44"/>
-      <c r="Q47" s="44"/>
-      <c r="R47" s="44"/>
-      <c r="S47" s="44"/>
+      <c r="O47" s="82"/>
+      <c r="P47" s="40"/>
+      <c r="Q47" s="40"/>
+      <c r="R47" s="40"/>
+      <c r="S47" s="40"/>
     </row>
     <row r="48" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G48" s="51"/>
+      <c r="G48" s="34"/>
       <c r="H48" s="14"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="45" t="s">
+      <c r="O48" s="82"/>
+      <c r="P48" s="80" t="s">
         <v>8</v>
       </c>
       <c r="Q48" s="23" t="s">
@@ -4848,30 +4905,30 @@
       </c>
     </row>
     <row r="49" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G49" s="51"/>
+      <c r="G49" s="34"/>
       <c r="H49" s="13"/>
-      <c r="O49" s="47"/>
-      <c r="P49" s="46"/>
+      <c r="O49" s="82"/>
+      <c r="P49" s="81"/>
       <c r="Q49" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="50" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G50" s="51"/>
+      <c r="G50" s="34"/>
       <c r="H50" s="14"/>
-      <c r="O50" s="47"/>
-      <c r="P50" s="46"/>
+      <c r="O50" s="82"/>
+      <c r="P50" s="81"/>
       <c r="Q50" s="24" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="51" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G51" s="51"/>
+      <c r="G51" s="34"/>
       <c r="H51" s="13"/>
-      <c r="O51" s="62" t="s">
+      <c r="O51" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="P51" s="48" t="s">
+      <c r="P51" s="83" t="s">
         <v>86</v>
       </c>
       <c r="Q51" s="25" t="s">
@@ -4879,94 +4936,94 @@
       </c>
     </row>
     <row r="52" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G52" s="51"/>
+      <c r="G52" s="34"/>
       <c r="H52" s="14"/>
-      <c r="O52" s="62"/>
-      <c r="P52" s="48"/>
+      <c r="O52" s="66"/>
+      <c r="P52" s="83"/>
       <c r="Q52" s="26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="53" spans="7:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G53" s="43" t="s">
+      <c r="G53" s="35" t="s">
         <v>19</v>
       </c>
       <c r="H53" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="O53" s="62"/>
-      <c r="P53" s="48"/>
+      <c r="O53" s="66"/>
+      <c r="P53" s="83"/>
       <c r="Q53" s="27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="54" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G54" s="43"/>
+      <c r="G54" s="35"/>
       <c r="H54" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="O54" s="62"/>
-      <c r="P54" s="34" t="s">
+      <c r="O54" s="66"/>
+      <c r="P54" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="Q54" s="49" t="s">
+      <c r="Q54" s="38" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="55" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G55" s="43"/>
+      <c r="G55" s="35"/>
       <c r="H55" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="O55" s="62"/>
-      <c r="P55" s="34"/>
-      <c r="Q55" s="49"/>
+      <c r="O55" s="66"/>
+      <c r="P55" s="75"/>
+      <c r="Q55" s="38"/>
     </row>
     <row r="56" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G56" s="43"/>
+      <c r="G56" s="35"/>
       <c r="H56" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="O56" s="62"/>
-      <c r="P56" s="34"/>
-      <c r="Q56" s="43" t="s">
+      <c r="O56" s="66"/>
+      <c r="P56" s="75"/>
+      <c r="Q56" s="35" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="57" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G57" s="43"/>
+      <c r="G57" s="35"/>
       <c r="H57" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="O57" s="62"/>
-      <c r="P57" s="34"/>
-      <c r="Q57" s="43"/>
+      <c r="O57" s="66"/>
+      <c r="P57" s="75"/>
+      <c r="Q57" s="35"/>
     </row>
     <row r="58" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G58" s="43"/>
+      <c r="G58" s="35"/>
       <c r="H58" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="O58" s="62"/>
-      <c r="P58" s="34"/>
+      <c r="O58" s="66"/>
+      <c r="P58" s="75"/>
     </row>
     <row r="59" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G59" s="43"/>
+      <c r="G59" s="35"/>
       <c r="H59" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="O59" s="62"/>
-      <c r="P59" s="34"/>
+      <c r="O59" s="66"/>
+      <c r="P59" s="75"/>
     </row>
     <row r="60" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G60" s="43"/>
+      <c r="G60" s="35"/>
       <c r="H60" s="18"/>
-      <c r="O60" s="62"/>
-      <c r="P60" s="34"/>
-      <c r="Q60" s="50" t="s">
+      <c r="O60" s="66"/>
+      <c r="P60" s="75"/>
+      <c r="Q60" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="R60" s="51" t="s">
+      <c r="R60" s="34" t="s">
         <v>93</v>
       </c>
       <c r="S60" s="23" t="s">
@@ -4980,14 +5037,14 @@
       </c>
     </row>
     <row r="61" spans="7:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G61" s="43"/>
-      <c r="H61" s="78" t="s">
+      <c r="G61" s="35"/>
+      <c r="H61" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="O61" s="62"/>
-      <c r="P61" s="34"/>
-      <c r="Q61" s="50"/>
-      <c r="R61" s="51"/>
+      <c r="O61" s="66"/>
+      <c r="P61" s="75"/>
+      <c r="Q61" s="84"/>
+      <c r="R61" s="34"/>
       <c r="S61" s="24" t="s">
         <v>111</v>
       </c>
@@ -5014,12 +5071,12 @@
       </c>
     </row>
     <row r="62" spans="7:26" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G62" s="43"/>
-      <c r="H62" s="79"/>
-      <c r="O62" s="62"/>
-      <c r="P62" s="34"/>
-      <c r="Q62" s="50"/>
-      <c r="R62" s="93" t="s">
+      <c r="G62" s="35"/>
+      <c r="H62" s="61"/>
+      <c r="O62" s="66"/>
+      <c r="P62" s="75"/>
+      <c r="Q62" s="84"/>
+      <c r="R62" s="51" t="s">
         <v>94</v>
       </c>
       <c r="S62" s="23" t="s">
@@ -5039,16 +5096,16 @@
       </c>
     </row>
     <row r="63" spans="7:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G63" s="41" t="s">
+      <c r="G63" s="58" t="s">
         <v>8</v>
       </c>
       <c r="H63" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="O63" s="62"/>
-      <c r="P63" s="34"/>
-      <c r="Q63" s="50"/>
-      <c r="R63" s="93"/>
+      <c r="O63" s="66"/>
+      <c r="P63" s="75"/>
+      <c r="Q63" s="84"/>
+      <c r="R63" s="51"/>
       <c r="S63" s="24" t="s">
         <v>113</v>
       </c>
@@ -5075,135 +5132,135 @@
       </c>
     </row>
     <row r="64" spans="7:26" x14ac:dyDescent="0.25">
-      <c r="G64" s="41"/>
+      <c r="G64" s="58"/>
       <c r="H64" s="21"/>
-      <c r="O64" s="62"/>
-      <c r="P64" s="34"/>
-      <c r="Q64" s="38" t="s">
+      <c r="O64" s="66"/>
+      <c r="P64" s="75"/>
+      <c r="Q64" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="R64" s="67" t="s">
+      <c r="R64" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="S64" s="67"/>
-      <c r="T64" s="67"/>
+      <c r="S64" s="72"/>
+      <c r="T64" s="72"/>
     </row>
     <row r="65" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G65" s="41"/>
+      <c r="G65" s="58"/>
       <c r="H65" s="21"/>
-      <c r="O65" s="62"/>
-      <c r="P65" s="34"/>
-      <c r="Q65" s="38"/>
-      <c r="R65" s="67"/>
-      <c r="S65" s="67"/>
-      <c r="T65" s="67"/>
+      <c r="O65" s="66"/>
+      <c r="P65" s="75"/>
+      <c r="Q65" s="46"/>
+      <c r="R65" s="72"/>
+      <c r="S65" s="72"/>
+      <c r="T65" s="72"/>
     </row>
     <row r="66" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G66" s="41"/>
+      <c r="G66" s="58"/>
       <c r="H66" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="O66" s="62"/>
-      <c r="P66" s="34"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="67"/>
-      <c r="S66" s="67"/>
-      <c r="T66" s="67"/>
+      <c r="O66" s="66"/>
+      <c r="P66" s="75"/>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="72"/>
+      <c r="S66" s="72"/>
+      <c r="T66" s="72"/>
     </row>
     <row r="67" spans="7:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G67" s="41"/>
+      <c r="G67" s="58"/>
       <c r="H67" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="O67" s="62"/>
-      <c r="P67" s="40" t="s">
+      <c r="O67" s="66"/>
+      <c r="P67" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="Q67" s="35" t="s">
+      <c r="Q67" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="R67" s="36" t="s">
+      <c r="R67" s="77" t="s">
         <v>153</v>
       </c>
-      <c r="S67" s="37" t="s">
+      <c r="S67" s="78" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="68" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G68" s="41"/>
+      <c r="G68" s="58"/>
       <c r="H68" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O68" s="62"/>
-      <c r="P68" s="40"/>
-      <c r="Q68" s="35"/>
-      <c r="R68" s="36"/>
-      <c r="S68" s="37"/>
+      <c r="O68" s="66"/>
+      <c r="P68" s="79"/>
+      <c r="Q68" s="76"/>
+      <c r="R68" s="77"/>
+      <c r="S68" s="78"/>
     </row>
     <row r="69" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G69" s="41"/>
+      <c r="G69" s="58"/>
       <c r="H69" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O69" s="62"/>
-      <c r="P69" s="40"/>
-      <c r="Q69" s="35"/>
-      <c r="R69" s="36"/>
-      <c r="S69" s="37"/>
+      <c r="O69" s="66"/>
+      <c r="P69" s="79"/>
+      <c r="Q69" s="76"/>
+      <c r="R69" s="77"/>
+      <c r="S69" s="78"/>
     </row>
     <row r="70" spans="7:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G70" s="41"/>
+      <c r="G70" s="58"/>
       <c r="H70" s="18"/>
-      <c r="O70" s="62"/>
-      <c r="P70" s="40"/>
-      <c r="Q70" s="38" t="s">
+      <c r="O70" s="66"/>
+      <c r="P70" s="79"/>
+      <c r="Q70" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="R70" s="39" t="s">
+      <c r="R70" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="S70" s="39"/>
-      <c r="T70" s="39"/>
-      <c r="U70" s="39"/>
-      <c r="V70" s="39"/>
+      <c r="S70" s="67"/>
+      <c r="T70" s="67"/>
+      <c r="U70" s="67"/>
+      <c r="V70" s="67"/>
     </row>
     <row r="71" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G71" s="51" t="s">
+      <c r="G71" s="34" t="s">
         <v>37</v>
       </c>
       <c r="H71" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="O71" s="62"/>
-      <c r="P71" s="40"/>
-      <c r="Q71" s="38"/>
-      <c r="R71" s="39"/>
-      <c r="S71" s="39"/>
-      <c r="T71" s="39"/>
-      <c r="U71" s="39"/>
-      <c r="V71" s="39"/>
+      <c r="O71" s="66"/>
+      <c r="P71" s="79"/>
+      <c r="Q71" s="46"/>
+      <c r="R71" s="67"/>
+      <c r="S71" s="67"/>
+      <c r="T71" s="67"/>
+      <c r="U71" s="67"/>
+      <c r="V71" s="67"/>
     </row>
     <row r="72" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G72" s="51"/>
+      <c r="G72" s="34"/>
       <c r="H72" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="O72" s="62"/>
-      <c r="P72" s="40"/>
-      <c r="Q72" s="38"/>
-      <c r="R72" s="39"/>
-      <c r="S72" s="39"/>
-      <c r="T72" s="39"/>
-      <c r="U72" s="39"/>
-      <c r="V72" s="39"/>
+      <c r="O72" s="66"/>
+      <c r="P72" s="79"/>
+      <c r="Q72" s="46"/>
+      <c r="R72" s="67"/>
+      <c r="S72" s="67"/>
+      <c r="T72" s="67"/>
+      <c r="U72" s="67"/>
+      <c r="V72" s="67"/>
     </row>
     <row r="73" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G73" s="51"/>
+      <c r="G73" s="34"/>
       <c r="H73" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="O73" s="62"/>
-      <c r="P73" s="63" t="s">
+      <c r="O73" s="66"/>
+      <c r="P73" s="68" t="s">
         <v>57</v>
       </c>
       <c r="Q73" s="7" t="s">
@@ -5211,116 +5268,116 @@
       </c>
     </row>
     <row r="74" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G74" s="41" t="s">
+      <c r="G74" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="82" t="s">
+      <c r="H74" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="O74" s="62"/>
-      <c r="P74" s="63"/>
+      <c r="O74" s="66"/>
+      <c r="P74" s="68"/>
       <c r="Q74" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="75" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G75" s="41"/>
-      <c r="H75" s="83"/>
-      <c r="O75" s="62"/>
-      <c r="P75" s="63"/>
-      <c r="Q75" s="38" t="s">
+      <c r="G75" s="58"/>
+      <c r="H75" s="49"/>
+      <c r="O75" s="66"/>
+      <c r="P75" s="68"/>
+      <c r="Q75" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="R75" s="39" t="s">
+      <c r="R75" s="67" t="s">
         <v>157</v>
       </c>
-      <c r="S75" s="39"/>
-      <c r="T75" s="39"/>
-      <c r="U75" s="39"/>
-      <c r="V75" s="39"/>
+      <c r="S75" s="67"/>
+      <c r="T75" s="67"/>
+      <c r="U75" s="67"/>
+      <c r="V75" s="67"/>
     </row>
     <row r="76" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G76" s="41"/>
-      <c r="H76" s="84" t="s">
+      <c r="G76" s="58"/>
+      <c r="H76" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="O76" s="62"/>
-      <c r="P76" s="63"/>
-      <c r="Q76" s="38"/>
-      <c r="R76" s="39"/>
-      <c r="S76" s="39"/>
-      <c r="T76" s="39"/>
-      <c r="U76" s="39"/>
-      <c r="V76" s="39"/>
+      <c r="O76" s="66"/>
+      <c r="P76" s="68"/>
+      <c r="Q76" s="46"/>
+      <c r="R76" s="67"/>
+      <c r="S76" s="67"/>
+      <c r="T76" s="67"/>
+      <c r="U76" s="67"/>
+      <c r="V76" s="67"/>
     </row>
     <row r="77" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G77" s="41"/>
-      <c r="H77" s="85"/>
-      <c r="O77" s="62"/>
-      <c r="P77" s="63"/>
-      <c r="Q77" s="38"/>
-      <c r="R77" s="39"/>
-      <c r="S77" s="39"/>
-      <c r="T77" s="39"/>
-      <c r="U77" s="39"/>
-      <c r="V77" s="39"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="65"/>
+      <c r="O77" s="66"/>
+      <c r="P77" s="68"/>
+      <c r="Q77" s="46"/>
+      <c r="R77" s="67"/>
+      <c r="S77" s="67"/>
+      <c r="T77" s="67"/>
+      <c r="U77" s="67"/>
+      <c r="V77" s="67"/>
     </row>
     <row r="78" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G78" s="41"/>
-      <c r="H78" s="82" t="s">
+      <c r="G78" s="58"/>
+      <c r="H78" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="P78" s="63"/>
-      <c r="Q78" s="66" t="s">
+      <c r="P78" s="68"/>
+      <c r="Q78" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="R78" s="64" t="s">
+      <c r="R78" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="S78" s="64"/>
-      <c r="T78" s="64"/>
+      <c r="S78" s="69"/>
+      <c r="T78" s="69"/>
     </row>
     <row r="79" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G79" s="41"/>
-      <c r="H79" s="83"/>
-      <c r="P79" s="63"/>
-      <c r="Q79" s="66"/>
-      <c r="R79" s="65" t="s">
+      <c r="G79" s="58"/>
+      <c r="H79" s="49"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="71"/>
+      <c r="R79" s="70" t="s">
         <v>160</v>
       </c>
-      <c r="S79" s="65"/>
-      <c r="T79" s="65"/>
+      <c r="S79" s="70"/>
+      <c r="T79" s="70"/>
     </row>
     <row r="80" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G80" s="41"/>
+      <c r="G80" s="58"/>
       <c r="H80" s="3"/>
-      <c r="Q80" s="66"/>
-      <c r="R80" s="92" t="s">
+      <c r="Q80" s="71"/>
+      <c r="R80" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="S80" s="92"/>
-      <c r="T80" s="92"/>
+      <c r="S80" s="50"/>
+      <c r="T80" s="50"/>
     </row>
     <row r="81" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G81" s="41"/>
+      <c r="G81" s="58"/>
       <c r="H81" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="82" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G82" s="41"/>
+      <c r="G82" s="58"/>
       <c r="H82" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="83" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G83" s="41"/>
+      <c r="G83" s="58"/>
       <c r="H83" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="84" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G84" s="43" t="s">
+      <c r="G84" s="35" t="s">
         <v>19</v>
       </c>
       <c r="H84" s="4" t="s">
@@ -5328,49 +5385,49 @@
       </c>
     </row>
     <row r="85" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G85" s="43"/>
+      <c r="G85" s="35"/>
       <c r="H85" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="86" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G86" s="43"/>
-      <c r="H86" s="77" t="s">
+      <c r="G86" s="35"/>
+      <c r="H86" s="59" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="87" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G87" s="43"/>
-      <c r="H87" s="77"/>
+      <c r="G87" s="35"/>
+      <c r="H87" s="59"/>
     </row>
     <row r="88" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G88" s="43"/>
+      <c r="G88" s="35"/>
       <c r="H88" s="18"/>
     </row>
     <row r="89" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G89" s="43"/>
-      <c r="H89" s="88" t="s">
+      <c r="G89" s="35"/>
+      <c r="H89" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="90" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G90" s="43"/>
-      <c r="H90" s="88"/>
+      <c r="G90" s="35"/>
+      <c r="H90" s="42"/>
     </row>
     <row r="91" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G91" s="43"/>
-      <c r="H91" s="88"/>
+      <c r="G91" s="35"/>
+      <c r="H91" s="42"/>
     </row>
     <row r="92" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G92" s="43"/>
-      <c r="H92" s="88"/>
+      <c r="G92" s="35"/>
+      <c r="H92" s="42"/>
     </row>
     <row r="93" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G93" s="43"/>
-      <c r="H93" s="89"/>
+      <c r="G93" s="35"/>
+      <c r="H93" s="43"/>
     </row>
     <row r="94" spans="7:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G94" s="51" t="s">
+      <c r="G94" s="34" t="s">
         <v>43</v>
       </c>
       <c r="H94" s="13" t="s">
@@ -5378,31 +5435,31 @@
       </c>
     </row>
     <row r="95" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G95" s="51"/>
+      <c r="G95" s="34"/>
       <c r="H95" s="4" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="96" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G96" s="51"/>
+      <c r="G96" s="34"/>
       <c r="H96" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="97" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G97" s="51"/>
+      <c r="G97" s="34"/>
       <c r="H97" s="4" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="98" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G98" s="51"/>
+      <c r="G98" s="34"/>
       <c r="H98" s="18" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="99" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G99" s="41" t="s">
+      <c r="G99" s="58" t="s">
         <v>8</v>
       </c>
       <c r="H99" s="24" t="s">
@@ -5410,54 +5467,54 @@
       </c>
     </row>
     <row r="100" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G100" s="41"/>
+      <c r="G100" s="58"/>
       <c r="H100" s="29" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="101" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G101" s="41"/>
+      <c r="G101" s="58"/>
       <c r="H101" s="29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="102" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G102" s="41"/>
+      <c r="G102" s="58"/>
       <c r="H102" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="103" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G103" s="75" t="s">
+      <c r="G103" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="H103" s="71" t="s">
+      <c r="H103" s="52" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="104" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G104" s="76"/>
-      <c r="H104" s="71"/>
+      <c r="G104" s="57"/>
+      <c r="H104" s="52"/>
     </row>
     <row r="105" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G105" s="76"/>
+      <c r="G105" s="57"/>
       <c r="H105" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="106" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G106" s="76"/>
-      <c r="H106" s="72" t="s">
+      <c r="G106" s="57"/>
+      <c r="H106" s="53" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="107" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G107" s="76"/>
-      <c r="H107" s="73"/>
+      <c r="G107" s="57"/>
+      <c r="H107" s="54"/>
     </row>
     <row r="108" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G108" s="76"/>
-      <c r="H108" s="74"/>
+      <c r="G108" s="57"/>
+      <c r="H108" s="55"/>
     </row>
     <row r="109" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G109" s="12"/>
@@ -5483,20 +5540,76 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="Z10:Z14"/>
-    <mergeCell ref="AA10:AC10"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="AA12:AC12"/>
-    <mergeCell ref="AA13:AC13"/>
-    <mergeCell ref="AA14:AC14"/>
-    <mergeCell ref="Z15:Z22"/>
-    <mergeCell ref="AA15:AA17"/>
-    <mergeCell ref="AB15:AB17"/>
-    <mergeCell ref="AC15:AC17"/>
-    <mergeCell ref="AA18:AC19"/>
-    <mergeCell ref="AA20:AA22"/>
-    <mergeCell ref="AB20:AB22"/>
-    <mergeCell ref="AC20:AC22"/>
+    <mergeCell ref="P54:P66"/>
+    <mergeCell ref="Q67:Q69"/>
+    <mergeCell ref="R67:R69"/>
+    <mergeCell ref="S67:S69"/>
+    <mergeCell ref="Q70:Q72"/>
+    <mergeCell ref="R70:V72"/>
+    <mergeCell ref="P67:P72"/>
+    <mergeCell ref="G74:G83"/>
+    <mergeCell ref="P38:P41"/>
+    <mergeCell ref="O24:O45"/>
+    <mergeCell ref="P46:S47"/>
+    <mergeCell ref="P48:P50"/>
+    <mergeCell ref="O46:O50"/>
+    <mergeCell ref="P51:P53"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="Q60:Q63"/>
+    <mergeCell ref="R60:R61"/>
+    <mergeCell ref="Q30:Q32"/>
+    <mergeCell ref="P33:P37"/>
+    <mergeCell ref="Q33:S37"/>
+    <mergeCell ref="Q42:S43"/>
+    <mergeCell ref="P42:P45"/>
+    <mergeCell ref="Q44:S45"/>
+    <mergeCell ref="O51:O77"/>
+    <mergeCell ref="Q75:Q77"/>
+    <mergeCell ref="R75:V77"/>
+    <mergeCell ref="P73:P79"/>
+    <mergeCell ref="R78:T78"/>
+    <mergeCell ref="R79:T79"/>
+    <mergeCell ref="Q78:Q80"/>
+    <mergeCell ref="R64:T66"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="B9:B18"/>
+    <mergeCell ref="S8:S10"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="S13:S15"/>
+    <mergeCell ref="P16:P18"/>
+    <mergeCell ref="Q16:Q18"/>
+    <mergeCell ref="R16:R18"/>
+    <mergeCell ref="Q8:Q10"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="P13:P15"/>
+    <mergeCell ref="Q13:Q15"/>
+    <mergeCell ref="R13:R15"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="G9:G18"/>
+    <mergeCell ref="H103:H104"/>
+    <mergeCell ref="H106:H108"/>
+    <mergeCell ref="G103:G108"/>
+    <mergeCell ref="G94:G98"/>
+    <mergeCell ref="G99:G102"/>
+    <mergeCell ref="G84:G93"/>
+    <mergeCell ref="G19:G24"/>
+    <mergeCell ref="H86:H87"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="G47:G52"/>
+    <mergeCell ref="G53:G62"/>
+    <mergeCell ref="G63:G70"/>
+    <mergeCell ref="G25:G34"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="G35:G46"/>
+    <mergeCell ref="G71:G73"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="H76:H77"/>
     <mergeCell ref="O1:R2"/>
     <mergeCell ref="O3:O7"/>
     <mergeCell ref="P3:R3"/>
@@ -5521,76 +5634,20 @@
     <mergeCell ref="R80:T80"/>
     <mergeCell ref="R62:R63"/>
     <mergeCell ref="Q64:Q66"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="G9:G18"/>
-    <mergeCell ref="H103:H104"/>
-    <mergeCell ref="H106:H108"/>
-    <mergeCell ref="G103:G108"/>
-    <mergeCell ref="G94:G98"/>
-    <mergeCell ref="G99:G102"/>
-    <mergeCell ref="G84:G93"/>
-    <mergeCell ref="G19:G24"/>
-    <mergeCell ref="H86:H87"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="G47:G52"/>
-    <mergeCell ref="G53:G62"/>
-    <mergeCell ref="G63:G70"/>
-    <mergeCell ref="G25:G34"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="G35:G46"/>
-    <mergeCell ref="G71:G73"/>
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="H76:H77"/>
-    <mergeCell ref="O51:O77"/>
-    <mergeCell ref="Q75:Q77"/>
-    <mergeCell ref="R75:V77"/>
-    <mergeCell ref="P73:P79"/>
-    <mergeCell ref="R78:T78"/>
-    <mergeCell ref="R79:T79"/>
-    <mergeCell ref="Q78:Q80"/>
-    <mergeCell ref="R64:T66"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="B9:B18"/>
-    <mergeCell ref="S8:S10"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="S13:S15"/>
-    <mergeCell ref="P16:P18"/>
-    <mergeCell ref="Q16:Q18"/>
-    <mergeCell ref="R16:R18"/>
-    <mergeCell ref="Q8:Q10"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="P13:P15"/>
-    <mergeCell ref="Q13:Q15"/>
-    <mergeCell ref="R13:R15"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="P54:P66"/>
-    <mergeCell ref="Q67:Q69"/>
-    <mergeCell ref="R67:R69"/>
-    <mergeCell ref="S67:S69"/>
-    <mergeCell ref="Q70:Q72"/>
-    <mergeCell ref="R70:V72"/>
-    <mergeCell ref="P67:P72"/>
-    <mergeCell ref="G74:G83"/>
-    <mergeCell ref="P38:P41"/>
-    <mergeCell ref="O24:O45"/>
-    <mergeCell ref="P46:S47"/>
-    <mergeCell ref="P48:P50"/>
-    <mergeCell ref="O46:O50"/>
-    <mergeCell ref="P51:P53"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q56:Q57"/>
-    <mergeCell ref="Q60:Q63"/>
-    <mergeCell ref="R60:R61"/>
-    <mergeCell ref="Q30:Q32"/>
-    <mergeCell ref="P33:P37"/>
-    <mergeCell ref="Q33:S37"/>
-    <mergeCell ref="Q42:S43"/>
-    <mergeCell ref="P42:P45"/>
-    <mergeCell ref="Q44:S45"/>
+    <mergeCell ref="Z10:Z14"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="AA12:AC12"/>
+    <mergeCell ref="AA13:AC13"/>
+    <mergeCell ref="AA14:AC14"/>
+    <mergeCell ref="Z15:Z22"/>
+    <mergeCell ref="AA15:AA17"/>
+    <mergeCell ref="AB15:AB17"/>
+    <mergeCell ref="AC15:AC17"/>
+    <mergeCell ref="AA18:AC19"/>
+    <mergeCell ref="AA20:AA22"/>
+    <mergeCell ref="AB20:AB22"/>
+    <mergeCell ref="AC20:AC22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5599,10 +5656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:AM20"/>
+  <dimension ref="D3:AO20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5610,7 +5667,7 @@
     <col min="1" max="16384" width="18.85546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:41" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="31" t="s">
         <v>17</v>
       </c>
@@ -5624,49 +5681,53 @@
         <v>163</v>
       </c>
       <c r="H3" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="I3" s="31" t="s">
         <v>199</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>200</v>
       </c>
       <c r="J3" s="31" t="s">
         <v>200</v>
       </c>
       <c r="K3" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="L3" s="31" t="s">
         <v>199</v>
-      </c>
-      <c r="L3" s="31" t="s">
-        <v>200</v>
       </c>
       <c r="M3" s="31" t="s">
         <v>200</v>
       </c>
       <c r="N3" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="O3" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="P3" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="O3" s="31" t="s">
+      <c r="Q3" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="R3" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="S3" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="T3" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="S3" s="31" t="s">
+      <c r="U3" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="T3" s="31" t="s">
+      <c r="V3" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="U3" s="31" t="s">
+      <c r="W3" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="V3"/>
-      <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
       <c r="Z3"/>
@@ -5683,8 +5744,10 @@
       <c r="AK3"/>
       <c r="AL3"/>
       <c r="AM3"/>
-    </row>
-    <row r="4" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="AN3"/>
+      <c r="AO3"/>
+    </row>
+    <row r="4" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D4" s="33">
         <v>1</v>
       </c>
@@ -5697,29 +5760,31 @@
       <c r="G4" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30">
+        <f>(10*3)/(14*3)</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I4" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="J4" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="K4" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="L4" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="M4" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="N4" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="N4" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>212</v>
+      <c r="O4" s="30">
+        <f>(4+3+5+5+4+4)/(5+5+6+5+6+5)</f>
+        <v>0.78125</v>
       </c>
       <c r="P4" s="33" t="s">
         <v>212</v>
@@ -5739,9 +5804,15 @@
       <c r="U4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="V4"/>
-    </row>
-    <row r="5" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V4" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="W4" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D5" s="32">
         <v>2</v>
       </c>
@@ -5754,29 +5825,31 @@
       <c r="G5" s="33" t="s">
         <v>229</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="30">
+        <f>(11+12+9)/(13*3)</f>
+        <v>0.82051282051282048</v>
+      </c>
+      <c r="I5" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="J5" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="K5" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="L5" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="M5" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="N5" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="N5" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>212</v>
+      <c r="O5" s="30">
+        <f>(4+4+6+5+5+4)/(5+5+6+5+5+5)</f>
+        <v>0.90322580645161288</v>
       </c>
       <c r="P5" s="32" t="s">
         <v>212</v>
@@ -5796,347 +5869,379 @@
       <c r="U5" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="V5"/>
-    </row>
-    <row r="6" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V5" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="W5" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="X5"/>
+    </row>
+    <row r="6" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D6" s="33">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="33" t="s">
+      <c r="E6" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" s="30">
+        <f>(11+11+13)/(14+15+14)</f>
+        <v>0.81395348837209303</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="N6" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="O6" s="30">
+        <f>(5+6+6+3+5+6)/(5+6+6+5+6+6)</f>
+        <v>0.91176470588235292</v>
+      </c>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="33"/>
       <c r="S6" s="32"/>
-      <c r="T6" s="33" t="s">
+      <c r="T6" s="33"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="U6" s="32"/>
-      <c r="V6"/>
-    </row>
-    <row r="7" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="W6" s="32"/>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D7" s="33">
         <v>4</v>
       </c>
       <c r="E7" s="33"/>
       <c r="F7" s="32"/>
       <c r="G7" s="33"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="32" t="s">
+      <c r="I7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="33"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="32"/>
       <c r="S7" s="33"/>
-      <c r="T7" s="32" t="s">
+      <c r="T7" s="32"/>
+      <c r="U7" s="33"/>
+      <c r="V7" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="U7" s="33"/>
-      <c r="V7"/>
-    </row>
-    <row r="8" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="W7" s="33"/>
+      <c r="X7"/>
+    </row>
+    <row r="8" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D8" s="32">
         <v>5</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="33"/>
       <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="32"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="32"/>
       <c r="P8" s="33"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="33"/>
       <c r="S8" s="32"/>
       <c r="T8" s="33"/>
       <c r="U8" s="32"/>
-    </row>
-    <row r="9" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V8" s="33"/>
+      <c r="W8" s="32"/>
+    </row>
+    <row r="9" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D9" s="33">
         <v>6</v>
       </c>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
       <c r="G9" s="33"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="33"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="33"/>
       <c r="P9" s="32"/>
       <c r="Q9" s="33"/>
       <c r="R9" s="32"/>
       <c r="S9" s="33"/>
       <c r="T9" s="32"/>
       <c r="U9" s="33"/>
-    </row>
-    <row r="10" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V9" s="32"/>
+      <c r="W9" s="33"/>
+    </row>
+    <row r="10" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D10" s="33">
         <v>7</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="33"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="32"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="32"/>
       <c r="P10" s="33"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="33"/>
       <c r="S10" s="32"/>
       <c r="T10" s="33"/>
       <c r="U10" s="32"/>
-    </row>
-    <row r="11" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V10" s="33"/>
+      <c r="W10" s="32"/>
+    </row>
+    <row r="11" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D11" s="32">
         <v>8</v>
       </c>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
       <c r="G11" s="33"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="33"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="33"/>
       <c r="P11" s="32"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="32"/>
       <c r="S11" s="33"/>
       <c r="T11" s="32"/>
       <c r="U11" s="33"/>
-    </row>
-    <row r="12" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V11" s="32"/>
+      <c r="W11" s="33"/>
+    </row>
+    <row r="12" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D12" s="33">
         <v>9</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="33"/>
       <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="32"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="33"/>
       <c r="S12" s="32"/>
       <c r="T12" s="33"/>
       <c r="U12" s="32"/>
-    </row>
-    <row r="13" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V12" s="33"/>
+      <c r="W12" s="32"/>
+    </row>
+    <row r="13" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D13" s="33">
         <v>10</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="33"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="33"/>
       <c r="P13" s="32"/>
       <c r="Q13" s="33"/>
       <c r="R13" s="32"/>
       <c r="S13" s="33"/>
       <c r="T13" s="32"/>
       <c r="U13" s="33"/>
-    </row>
-    <row r="14" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V13" s="32"/>
+      <c r="W13" s="33"/>
+    </row>
+    <row r="14" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D14" s="32">
         <v>11</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="33"/>
       <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
+      <c r="N14" s="32"/>
       <c r="P14" s="33"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="33"/>
       <c r="S14" s="32"/>
       <c r="T14" s="33"/>
       <c r="U14" s="32"/>
-    </row>
-    <row r="15" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V14" s="33"/>
+      <c r="W14" s="32"/>
+    </row>
+    <row r="15" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D15" s="33">
         <v>12</v>
       </c>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="33"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="33"/>
       <c r="P15" s="32"/>
       <c r="Q15" s="33"/>
       <c r="R15" s="32"/>
       <c r="S15" s="33"/>
       <c r="T15" s="32"/>
       <c r="U15" s="33"/>
-    </row>
-    <row r="16" spans="4:39" x14ac:dyDescent="0.25">
+      <c r="V15" s="32"/>
+      <c r="W15" s="33"/>
+    </row>
+    <row r="16" spans="4:41" x14ac:dyDescent="0.25">
       <c r="D16" s="33">
         <v>13</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="33"/>
       <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="32"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="32"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="33"/>
       <c r="S16" s="32"/>
       <c r="T16" s="33"/>
       <c r="U16" s="32"/>
-    </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="33"/>
+      <c r="W16" s="32"/>
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D17" s="32">
         <v>14</v>
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="33"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="33"/>
       <c r="P17" s="32"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="32"/>
       <c r="S17" s="33"/>
       <c r="T17" s="32"/>
       <c r="U17" s="33"/>
-    </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="32"/>
+      <c r="W17" s="33"/>
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D18" s="33">
         <v>15</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="33"/>
       <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="32"/>
       <c r="P18" s="33"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="33"/>
       <c r="S18" s="32"/>
       <c r="T18" s="33"/>
       <c r="U18" s="32"/>
-    </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="33"/>
+      <c r="W18" s="32"/>
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D19" s="33">
         <v>16</v>
       </c>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="33"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="33"/>
       <c r="P19" s="32"/>
       <c r="Q19" s="33"/>
       <c r="R19" s="32"/>
       <c r="S19" s="33"/>
       <c r="T19" s="32"/>
       <c r="U19" s="33"/>
-    </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="32"/>
+      <c r="W19" s="33"/>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D20" s="32">
         <v>17</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
       <c r="G20" s="32"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="32"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="32"/>
       <c r="P20" s="33"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="33"/>
       <c r="S20" s="32"/>
       <c r="T20" s="33"/>
       <c r="U20" s="32"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6148,8 +6253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6335,25 +6440,45 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
@@ -6497,5 +6622,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>